<commit_message>
Making searchable recipies based on ingredients
</commit_message>
<xml_diff>
--- a/Directions.xlsx
+++ b/Directions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t xml:space="preserve">Recipe</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Quinoa Veggie Bowl</t>
   </si>
   <si>
-    <t xml:space="preserve">Claire Borchers</t>
+    <t xml:space="preserve">Claire B</t>
   </si>
   <si>
     <t xml:space="preserve">Put all in a rice cooker or cook quinoa and veggies seperately then add everything together</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Chewy Oatmeal Cookies</t>
   </si>
   <si>
-    <t xml:space="preserve">Claire Cantlon</t>
+    <t xml:space="preserve">Claire C</t>
   </si>
   <si>
     <t xml:space="preserve">Mix and bake at 350F deg for 10 minutes</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Chicken Noodle Soup</t>
   </si>
   <si>
-    <t xml:space="preserve">Mitchell Borchers</t>
+    <t xml:space="preserve">Mitchell B</t>
   </si>
   <si>
     <t xml:space="preserve">Pour borth in pot, cut up veggies and put in broth, put chicken in broth, bring to boil and put noodles in, season to taste, boil until chicken and noodles cooked, pull apart chicken and put back in soup</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Crustless Quiche</t>
   </si>
   <si>
-    <t xml:space="preserve">Mum Borchers</t>
+    <t xml:space="preserve">Mum B</t>
   </si>
   <si>
     <t xml:space="preserve">Create egg and cream mixture with spices, spray pan, thin walled baking pan preffered. Bake at 325 for 25-30 minutes</t>
@@ -85,10 +85,13 @@
     <t xml:space="preserve">Zuchinni Bread</t>
   </si>
   <si>
+    <t xml:space="preserve">TBD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Turkey Trot Meatballs</t>
   </si>
   <si>
-    <t xml:space="preserve">Shalane</t>
+    <t xml:space="preserve">Shalane F</t>
   </si>
   <si>
     <t xml:space="preserve">Oven to 400F, baking sheet with parchment paper with oil on top, combine ingreds and let rest for 15 mins, bake for 30 mins, flip halfway thru</t>
@@ -145,6 +148,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -254,7 +258,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -320,7 +324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -349,90 +353,96 @@
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>